<commit_message>
Implement comp reference for clubs
</commit_message>
<xml_diff>
--- a/clubs.xlsx
+++ b/clubs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="203">
   <si>
     <t>Full Name</t>
   </si>
@@ -51,10 +51,10 @@
     <t>Titlebar BG (Hex)</t>
   </si>
   <si>
-    <t>Division DBID</t>
-  </si>
-  <si>
-    <t>Last Division DBID</t>
+    <t>Division Name (Or DBID)</t>
+  </si>
+  <si>
+    <t>Last Division Name (Or DBID)</t>
   </si>
   <si>
     <t>Test Boldklub</t>
@@ -75,6 +75,12 @@
     <t>#000000</t>
   </si>
   <si>
+    <t>2000170400</t>
+  </si>
+  <si>
+    <t>Copenhagen, Series 1</t>
+  </si>
+  <si>
     <t>Handel Boldklub</t>
   </si>
   <si>
@@ -87,6 +93,9 @@
     <t>#f44336</t>
   </si>
   <si>
+    <t>932444</t>
+  </si>
+  <si>
     <t>Club1</t>
   </si>
   <si>
@@ -102,6 +111,9 @@
     <t>#741b47</t>
   </si>
   <si>
+    <t>Jutland, Series 5</t>
+  </si>
+  <si>
     <t>Club2</t>
   </si>
   <si>
@@ -129,6 +141,9 @@
     <t>S3A</t>
   </si>
   <si>
+    <t>Zealand, Series 1</t>
+  </si>
+  <si>
     <t>Club4</t>
   </si>
   <si>
@@ -399,15 +414,9 @@
     <t>BS</t>
   </si>
   <si>
-    <t>Copenhagen, Series 1</t>
-  </si>
-  <si>
     <t>CS1</t>
   </si>
   <si>
-    <t>Zealand, Series 1</t>
-  </si>
-  <si>
     <t>ZS1</t>
   </si>
   <si>
@@ -562,9 +571,6 @@
   </si>
   <si>
     <t>FS5</t>
-  </si>
-  <si>
-    <t>Jutland, Series 5</t>
   </si>
   <si>
     <t>JS5</t>
@@ -655,18 +661,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,8 +788,8 @@
     <tableColumn name="Reputation" id="8"/>
     <tableColumn name="Titlebar FG (Hex)" id="9"/>
     <tableColumn name="Titlebar BG (Hex)" id="10"/>
-    <tableColumn name="Division DBID" id="11"/>
-    <tableColumn name="Last Division DBID" id="12"/>
+    <tableColumn name="Division Name (Or DBID)" id="11"/>
+    <tableColumn name="Last Division Name (Or DBID)" id="12"/>
   </tableColumns>
   <tableStyleInfo name="Clubs-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -1016,8 +1034,11 @@
     <col customWidth="1" min="4" max="4" width="14.57"/>
     <col customWidth="1" min="5" max="5" width="16.86"/>
     <col customWidth="1" min="6" max="6" width="13.29"/>
-    <col customWidth="1" min="7" max="7" width="16.43"/>
-    <col customWidth="1" min="8" max="12" width="15.86"/>
+    <col customWidth="1" min="7" max="7" width="15.43"/>
+    <col customWidth="1" min="8" max="8" width="10.71"/>
+    <col customWidth="1" min="9" max="10" width="15.86"/>
+    <col customWidth="1" min="11" max="11" width="21.86"/>
+    <col customWidth="1" min="12" max="12" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1077,7 +1098,7 @@
       <c r="F2" s="2">
         <v>1949.0</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H2" s="2">
@@ -1089,33 +1110,33 @@
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L2" s="1">
-        <v>932444.0</v>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2">
         <v>1912.0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <v>70.0</v>
       </c>
       <c r="H3" s="2">
@@ -1125,35 +1146,35 @@
         <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L3" s="1">
-        <v>932444.0</v>
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2">
         <v>1875.0</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H4" s="2">
@@ -1163,35 +1184,35 @@
         <v>16</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L4" s="1">
-        <v>932444.0</v>
+        <v>29</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2">
         <v>1838.0</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H5" s="2">
@@ -1201,35 +1222,35 @@
         <v>16</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L5" s="1">
-        <v>932444.0</v>
+        <v>35</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2">
         <v>1801.0</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H6" s="2">
@@ -1241,33 +1262,33 @@
       <c r="J6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L6" s="1">
-        <v>932444.0</v>
+      <c r="K6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2">
         <v>1764.0</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H7" s="2">
@@ -1279,33 +1300,33 @@
       <c r="J7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L7" s="1">
-        <v>932444.0</v>
+      <c r="K7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2">
         <v>1727.0</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H8" s="2">
@@ -1317,33 +1338,33 @@
       <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L8" s="1">
-        <v>932444.0</v>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2">
         <v>1690.0</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H9" s="2">
@@ -1355,33 +1376,33 @@
       <c r="J9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L9" s="1">
-        <v>932444.0</v>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2">
         <v>1653.0</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H10" s="2">
@@ -1393,33 +1414,33 @@
       <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L10" s="1">
-        <v>932444.0</v>
+      <c r="K10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F11" s="2">
         <v>1616.0</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H11" s="2">
@@ -1431,33 +1452,33 @@
       <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L11" s="1">
-        <v>932444.0</v>
+      <c r="K11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2">
         <v>1579.0</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H12" s="2">
@@ -1469,33 +1490,33 @@
       <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L12" s="1">
-        <v>932444.0</v>
+      <c r="K12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F13" s="2">
         <v>1542.0</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H13" s="2">
@@ -1507,33 +1528,33 @@
       <c r="J13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L13" s="1">
-        <v>932444.0</v>
+      <c r="K13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2">
         <v>1505.0</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H14" s="2">
@@ -1545,33 +1566,33 @@
       <c r="J14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L14" s="1">
-        <v>932444.0</v>
+      <c r="K14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2">
         <v>1468.0</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H15" s="2">
@@ -1583,33 +1604,33 @@
       <c r="J15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L15" s="1">
-        <v>932444.0</v>
+      <c r="K15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F16" s="2">
         <v>1431.0</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H16" s="2">
@@ -1621,33 +1642,33 @@
       <c r="J16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L16" s="1">
-        <v>932444.0</v>
+      <c r="K16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F17" s="2">
         <v>1394.0</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H17" s="2">
@@ -1659,33 +1680,33 @@
       <c r="J17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L17" s="1">
-        <v>932444.0</v>
+      <c r="K17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2">
         <v>1357.0</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H18" s="2">
@@ -1697,33 +1718,33 @@
       <c r="J18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L18" s="1">
-        <v>932444.0</v>
+      <c r="K18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F19" s="2">
         <v>1320.0</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H19" s="2">
@@ -1735,33 +1756,33 @@
       <c r="J19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L19" s="1">
-        <v>932444.0</v>
+      <c r="K19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F20" s="2">
         <v>1283.0</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H20" s="2">
@@ -1773,33 +1794,33 @@
       <c r="J20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L20" s="1">
-        <v>932444.0</v>
+      <c r="K20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F21" s="2">
         <v>1246.0</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H21" s="2">
@@ -1811,33 +1832,33 @@
       <c r="J21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L21" s="1">
-        <v>932444.0</v>
+      <c r="K21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F22" s="2">
         <v>1209.0</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H22" s="2">
@@ -1849,33 +1870,33 @@
       <c r="J22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L22" s="1">
-        <v>932444.0</v>
+      <c r="K22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F23" s="2">
         <v>1172.0</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H23" s="2">
@@ -1887,33 +1908,33 @@
       <c r="J23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L23" s="1">
-        <v>932444.0</v>
+      <c r="K23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F24" s="2">
         <v>1135.0</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H24" s="2">
@@ -1925,33 +1946,33 @@
       <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L24" s="1">
-        <v>932444.0</v>
+      <c r="K24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F25" s="2">
         <v>1098.0</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H25" s="2">
@@ -1963,33 +1984,33 @@
       <c r="J25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L25" s="1">
-        <v>932444.0</v>
+      <c r="K25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F26" s="2">
         <v>1061.0</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H26" s="2">
@@ -2001,33 +2022,33 @@
       <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L26" s="1">
-        <v>932444.0</v>
+      <c r="K26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F27" s="2">
         <v>1024.0</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H27" s="2">
@@ -2039,33 +2060,33 @@
       <c r="J27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L27" s="1">
-        <v>932444.0</v>
+      <c r="K27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F28" s="2">
         <v>987.0</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H28" s="2">
@@ -2077,33 +2098,33 @@
       <c r="J28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L28" s="1">
-        <v>932444.0</v>
+      <c r="K28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F29" s="2">
         <v>950.0</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H29" s="2">
@@ -2115,33 +2136,33 @@
       <c r="J29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L29" s="1">
-        <v>932444.0</v>
+      <c r="K29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F30" s="2">
         <v>913.0</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H30" s="2">
@@ -2153,33 +2174,33 @@
       <c r="J30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L30" s="1">
-        <v>932444.0</v>
+      <c r="K30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F31" s="2">
         <v>876.0</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H31" s="2">
@@ -2191,33 +2212,33 @@
       <c r="J31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L31" s="1">
-        <v>932444.0</v>
+      <c r="K31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F32" s="2">
         <v>839.0</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="3">
         <v>2.000020652E9</v>
       </c>
       <c r="H32" s="2">
@@ -2229,33 +2250,33 @@
       <c r="J32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="1">
-        <v>2.0001704E9</v>
-      </c>
-      <c r="L32" s="1">
-        <v>932444.0</v>
+      <c r="K32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F33" s="2">
         <v>802.0</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="3">
         <v>146.0</v>
       </c>
       <c r="H33" s="2">
@@ -2267,11 +2288,11 @@
       <c r="J33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="1">
-        <v>932444.0</v>
-      </c>
-      <c r="L33" s="1">
-        <v>2.0001704E9</v>
+      <c r="K33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2304,702 +2325,702 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>120</v>
+      <c r="F1" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="2">
+        <v>127</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="6">
         <v>11.0</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="7">
         <v>7.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>125</v>
+      <c r="A3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="2">
+        <v>126</v>
+      </c>
+      <c r="E3" s="6">
         <v>11.0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="7">
         <v>7.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="E4" s="6">
         <v>11.0</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="7">
         <v>7.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" s="2">
+        <v>126</v>
+      </c>
+      <c r="E5" s="6">
         <v>11.0</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="7">
         <v>7.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>131</v>
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="2">
+        <v>126</v>
+      </c>
+      <c r="E6" s="6">
         <v>11.0</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="7">
         <v>7.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E7" s="2">
+        <v>126</v>
+      </c>
+      <c r="E7" s="6">
         <v>11.0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="7">
         <v>7.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E8" s="2">
+        <v>126</v>
+      </c>
+      <c r="E8" s="6">
         <v>7.0</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="7">
         <v>8.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="2">
+        <v>140</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="6">
         <v>7.0</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="7">
         <v>8.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="E10" s="6">
         <v>7.0</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="7">
         <v>8.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" s="2">
+        <v>139</v>
+      </c>
+      <c r="E11" s="6">
         <v>7.0</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="7">
         <v>8.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" s="2">
+        <v>139</v>
+      </c>
+      <c r="E12" s="6">
         <v>7.0</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="7">
         <v>8.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" s="2">
+        <v>139</v>
+      </c>
+      <c r="E13" s="6">
         <v>7.0</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="7">
         <v>8.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="2">
+        <v>139</v>
+      </c>
+      <c r="E14" s="6">
         <v>7.0</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="7">
         <v>8.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E15" s="2">
+        <v>139</v>
+      </c>
+      <c r="E15" s="6">
         <v>7.0</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="7">
         <v>8.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="2">
+        <v>154</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="6">
         <v>5.0</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="7">
         <v>9.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="E17" s="6">
         <v>5.0</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="7">
         <v>9.0</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="2">
+        <v>153</v>
+      </c>
+      <c r="E18" s="6">
         <v>5.0</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="7">
         <v>9.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" s="2">
+        <v>153</v>
+      </c>
+      <c r="E19" s="6">
         <v>5.0</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="7">
         <v>9.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E20" s="2">
+        <v>153</v>
+      </c>
+      <c r="E20" s="6">
         <v>5.0</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="7">
         <v>9.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" s="2">
+        <v>153</v>
+      </c>
+      <c r="E21" s="6">
         <v>5.0</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="7">
         <v>9.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="2">
+        <v>166</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="6">
         <v>3.0</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="7">
         <v>10.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="E23" s="6">
         <v>3.0</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="7">
         <v>10.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="2">
+        <v>165</v>
+      </c>
+      <c r="E24" s="6">
         <v>3.0</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="7">
         <v>10.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="2">
+        <v>165</v>
+      </c>
+      <c r="E25" s="6">
         <v>3.0</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="7">
         <v>10.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E26" s="2">
+        <v>165</v>
+      </c>
+      <c r="E26" s="6">
         <v>3.0</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="7">
         <v>10.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E27" s="2">
+        <v>165</v>
+      </c>
+      <c r="E27" s="6">
         <v>3.0</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="7">
         <v>10.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E28" s="2">
+        <v>177</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="6">
         <v>2.0</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="7">
         <v>11.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="E29" s="6">
         <v>2.0</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="7">
         <v>11.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E30" s="2">
+        <v>176</v>
+      </c>
+      <c r="E30" s="6">
         <v>2.0</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="7">
         <v>11.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E31" s="2">
+        <v>176</v>
+      </c>
+      <c r="E31" s="6">
         <v>2.0</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="7">
         <v>11.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>181</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>181</v>
+        <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="2">
+        <v>176</v>
+      </c>
+      <c r="E32" s="6">
         <v>2.0</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="7">
         <v>11.0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" s="2">
+        <v>186</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="6">
         <v>1.0</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="7">
         <v>12.0</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="E34" s="6">
         <v>1.0</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="7">
         <v>12.0</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E35" s="2">
+        <v>185</v>
+      </c>
+      <c r="E35" s="6">
         <v>1.0</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="7">
         <v>12.0</v>
       </c>
     </row>
@@ -3033,153 +3054,153 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>194</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="str">
+      <c r="A2" s="5" t="str">
         <f t="shared" ref="A2:A4" si="1">#REF!+ROW(A2)-1</f>
         <v>#REF!</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E2" s="3">
+      <c r="C2" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="6">
         <v>55803.0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
         <v>11443.0</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="5">
         <v>21.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="str">
+      <c r="A3" s="5" t="str">
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="6">
         <v>55786.0</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
         <v>11468.0</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="5">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="str">
+      <c r="A4" s="5" t="str">
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="B4" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" s="6">
         <v>58823.0</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>11403.0</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <v>36.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>

<commit_message>
Stadium creation mostly implemented
</commit_message>
<xml_diff>
--- a/clubs.xlsx
+++ b/clubs.xlsx
@@ -12,7 +12,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mghLFSFcc0StyQrl+JpXTn+cVdkfQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mgeNrzjr/vYm/CF5JcJtUNdZqIHbg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -43,14 +43,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgukTcYY2Sp+6XYypuv6JvT0fQI/Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhrNfoYTfTzxcoza2TcVOBURBM66A=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="167">
   <si>
     <t>Full Name</t>
   </si>
@@ -496,9 +496,6 @@
     <t>Owner Type</t>
   </si>
   <si>
-    <t>Orientation</t>
-  </si>
-  <si>
     <t>Capacity</t>
   </si>
   <si>
@@ -521,6 +518,39 @@
   </si>
   <si>
     <t>Environment</t>
+  </si>
+  <si>
+    <t>Test Stadium</t>
+  </si>
+  <si>
+    <t>Council</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Stadium 2</t>
+  </si>
+  <si>
+    <t>Synthetic (New Type - Soft)</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>Basic</t>
   </si>
 </sst>
 </file>
@@ -569,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -612,11 +642,8 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,21 +790,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:M3" displayName="Table_4" id="4">
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L3" displayName="Table_4" id="4">
+  <tableColumns count="12">
     <tableColumn name="Name" id="1"/>
     <tableColumn name="Owner Type" id="2"/>
     <tableColumn name="Latitude" id="3"/>
     <tableColumn name="Longitude" id="4"/>
-    <tableColumn name="Orientation" id="5"/>
-    <tableColumn name="Capacity" id="6"/>
-    <tableColumn name="Seat  Capacity" id="7"/>
-    <tableColumn name="Pitch Type" id="8"/>
-    <tableColumn name="Pitch Condition" id="9"/>
-    <tableColumn name="Pitch Deterioration Rate" id="10"/>
-    <tableColumn name="Pitch Recovery Rate" id="11"/>
-    <tableColumn name="Stadium Condition" id="12"/>
-    <tableColumn name="Environment" id="13"/>
+    <tableColumn name="Capacity" id="5"/>
+    <tableColumn name="Seat  Capacity" id="6"/>
+    <tableColumn name="Pitch Type" id="7"/>
+    <tableColumn name="Pitch Condition" id="8"/>
+    <tableColumn name="Pitch Deterioration Rate" id="9"/>
+    <tableColumn name="Pitch Recovery Rate" id="10"/>
+    <tableColumn name="Stadium Condition" id="11"/>
+    <tableColumn name="Environment" id="12"/>
   </tableColumns>
   <tableStyleInfo name="Stadiums-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -2406,14 +2432,14 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="23.29"/>
-    <col customWidth="1" min="2" max="5" width="19.57"/>
-    <col customWidth="1" min="6" max="6" width="14.57"/>
-    <col customWidth="1" min="7" max="7" width="13.86"/>
-    <col customWidth="1" min="8" max="8" width="15.71"/>
-    <col customWidth="1" min="9" max="9" width="13.86"/>
-    <col customWidth="1" min="10" max="10" width="21.57"/>
-    <col customWidth="1" min="11" max="12" width="20.57"/>
-    <col customWidth="1" min="13" max="13" width="15.57"/>
+    <col customWidth="1" min="2" max="4" width="19.57"/>
+    <col customWidth="1" min="5" max="5" width="14.57"/>
+    <col customWidth="1" min="6" max="6" width="13.86"/>
+    <col customWidth="1" min="7" max="7" width="24.29"/>
+    <col customWidth="1" min="8" max="8" width="13.86"/>
+    <col customWidth="1" min="9" max="9" width="21.57"/>
+    <col customWidth="1" min="10" max="11" width="20.57"/>
+    <col customWidth="1" min="12" max="12" width="15.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
@@ -2453,39 +2479,82 @@
       <c r="L1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="6" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="8"/>
+      <c r="B2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="14">
+        <v>55.231</v>
+      </c>
+      <c r="D2" s="14">
+        <v>10.443</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1000.0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="6">
+        <v>80.0</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="8">
+        <v>110.0</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="8"/>
+      <c r="A3" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="14">
+        <v>55.33131</v>
+      </c>
+      <c r="D3" s="14">
+        <v>10.51113</v>
+      </c>
+      <c r="E3" s="6">
+        <v>750.0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H3" s="6">
+        <v>120.0</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="J3" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>

<commit_message>
Change colors to be set based on cell background color
</commit_message>
<xml_diff>
--- a/clubs.xlsx
+++ b/clubs.xlsx
@@ -12,7 +12,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mghLFSFcc0StyQrl+JpXTn+cVdkfQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhyj7qPFZAiGnki/VqkvQL8MtbTyg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="169">
   <si>
     <t>Full Name</t>
   </si>
@@ -79,10 +79,10 @@
     <t>Reputation</t>
   </si>
   <si>
-    <t>Titlebar FG (Hex)</t>
-  </si>
-  <si>
-    <t>Titlebar BG (Hex)</t>
+    <t>Titlebar FG</t>
+  </si>
+  <si>
+    <t>Titlebar BG</t>
   </si>
   <si>
     <t>Division Name/DBID</t>
@@ -91,6 +91,24 @@
     <t>Last Division Name/DBID</t>
   </si>
   <si>
+    <t>Home Kit Type</t>
+  </si>
+  <si>
+    <t>Home Kit FG</t>
+  </si>
+  <si>
+    <t>Home Kit BG</t>
+  </si>
+  <si>
+    <t>Away Kit Type</t>
+  </si>
+  <si>
+    <t>Away Kit FG</t>
+  </si>
+  <si>
+    <t>Away Kit BG</t>
+  </si>
+  <si>
     <t>Test Boldklub</t>
   </si>
   <si>
@@ -109,12 +127,6 @@
     <t>Test Stadium</t>
   </si>
   <si>
-    <t>#FFFFFF</t>
-  </si>
-  <si>
-    <t>#000000</t>
-  </si>
-  <si>
     <t>2000170400</t>
   </si>
   <si>
@@ -136,9 +148,6 @@
     <t>Stadium 2</t>
   </si>
   <si>
-    <t>#f44336</t>
-  </si>
-  <si>
     <t>932444</t>
   </si>
   <si>
@@ -160,9 +169,6 @@
     <t>933962</t>
   </si>
   <si>
-    <t>#741b47</t>
-  </si>
-  <si>
     <t>Jutland, Series 5</t>
   </si>
   <si>
@@ -176,9 +182,6 @@
   </si>
   <si>
     <t>S2A</t>
-  </si>
-  <si>
-    <t>#6aa84f</t>
   </si>
   <si>
     <t>Club3</t>
@@ -576,7 +579,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,8 +588,44 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF44336"/>
+        <bgColor rgb="FFF44336"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDEEAF6"/>
         <bgColor rgb="FFDEEAF6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF741B47"/>
+        <bgColor rgb="FF741B47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A86E8"/>
+        <bgColor rgb="FF4A86E8"/>
       </patternFill>
     </fill>
     <fill>
@@ -602,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -615,10 +654,28 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -630,19 +687,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -743,8 +800,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:M13" displayName="Table_1" id="1">
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:S13" displayName="Table_1" id="1">
+  <tableColumns count="19">
     <tableColumn name="Full Name" id="1"/>
     <tableColumn name="Short Name" id="2"/>
     <tableColumn name="6-Letter Name" id="3"/>
@@ -754,10 +811,16 @@
     <tableColumn name="City Name/DBID" id="7"/>
     <tableColumn name="Stadium Name/DBID" id="8"/>
     <tableColumn name="Reputation" id="9"/>
-    <tableColumn name="Titlebar FG (Hex)" id="10"/>
-    <tableColumn name="Titlebar BG (Hex)" id="11"/>
+    <tableColumn name="Titlebar FG" id="10"/>
+    <tableColumn name="Titlebar BG" id="11"/>
     <tableColumn name="Division Name/DBID" id="12"/>
     <tableColumn name="Last Division Name/DBID" id="13"/>
+    <tableColumn name="Home Kit Type" id="14"/>
+    <tableColumn name="Home Kit FG" id="15"/>
+    <tableColumn name="Home Kit BG" id="16"/>
+    <tableColumn name="Away Kit Type" id="17"/>
+    <tableColumn name="Away Kit FG" id="18"/>
+    <tableColumn name="Away Kit BG" id="19"/>
   </tableColumns>
   <tableStyleInfo name="Clubs-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -1019,16 +1082,22 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="26.14"/>
     <col customWidth="1" min="2" max="2" width="16.14"/>
-    <col customWidth="1" min="3" max="3" width="19.57"/>
-    <col customWidth="1" min="4" max="4" width="14.57"/>
-    <col customWidth="1" min="5" max="5" width="16.86"/>
-    <col customWidth="1" min="6" max="6" width="13.29"/>
-    <col customWidth="1" min="7" max="7" width="15.43"/>
-    <col customWidth="1" min="8" max="8" width="18.86"/>
-    <col customWidth="1" min="9" max="9" width="10.71"/>
-    <col customWidth="1" min="10" max="11" width="15.86"/>
+    <col customWidth="1" min="3" max="4" width="12.57"/>
+    <col customWidth="1" min="5" max="5" width="15.43"/>
+    <col customWidth="1" min="6" max="6" width="12.0"/>
+    <col customWidth="1" min="7" max="7" width="16.29"/>
+    <col customWidth="1" min="8" max="8" width="17.86"/>
+    <col customWidth="1" min="9" max="9" width="9.57"/>
+    <col customWidth="1" min="10" max="10" width="9.71"/>
+    <col customWidth="1" min="11" max="11" width="9.86"/>
     <col customWidth="1" min="12" max="12" width="19.57"/>
-    <col customWidth="1" min="13" max="13" width="25.29"/>
+    <col customWidth="1" min="13" max="13" width="21.57"/>
+    <col customWidth="1" min="14" max="14" width="13.14"/>
+    <col customWidth="1" min="15" max="15" width="11.57"/>
+    <col customWidth="1" min="16" max="16" width="11.71"/>
+    <col customWidth="1" min="17" max="17" width="12.71"/>
+    <col customWidth="1" min="18" max="18" width="10.86"/>
+    <col customWidth="1" min="19" max="19" width="11.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1071,498 +1140,540 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2">
         <v>1949.0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2">
         <v>150.0</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2">
         <v>1912.0</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="3">
+        <v>300.0</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="2">
-        <v>850.0</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2">
         <v>1875.0</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>34</v>
+      <c r="G4" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1550.0</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2000.0</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2">
         <v>1838.0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="2">
-        <v>2250.0</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I5" s="3">
+        <v>250.0</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="9"/>
       <c r="L5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2">
         <v>1801.0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="2">
-        <v>2950.0</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I6" s="3">
+        <v>95.0</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F7" s="2">
         <v>1764.0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="2">
-        <v>3650.0</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I7" s="3">
+        <v>90.0</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F8" s="2">
         <v>1727.0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="2">
-        <v>4350.0</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I8" s="3">
+        <v>80.0</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="6"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2">
         <v>1690.0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="2">
-        <v>5050.0</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I9" s="3">
+        <v>78.0</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="6"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" s="2">
         <v>1653.0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="2">
-        <v>5750.0</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I10" s="3">
+        <v>200.0</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="5"/>
       <c r="L10" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="6"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2">
         <v>1616.0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="2">
-        <v>6450.0</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I11" s="3">
+        <v>120.0</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="5"/>
       <c r="L11" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="9"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F12" s="2">
         <v>1579.0</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>66</v>
+      <c r="G12" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="2">
-        <v>7150.0</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I12" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="5"/>
       <c r="L12" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="9"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F13" s="2">
         <v>1542.0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="2">
-        <v>7850.0</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I13" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="9"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -1594,702 +1705,702 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>71</v>
+      <c r="C1" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>73</v>
+      <c r="F1" s="12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="13">
+        <v>11.0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="E3" s="13">
         <v>11.0</v>
       </c>
-      <c r="F2" s="8">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="7">
-        <v>11.0</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="F3" s="14">
         <v>7.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="7">
+        <v>75</v>
+      </c>
+      <c r="E4" s="13">
         <v>11.0</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="14">
         <v>7.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="7">
+        <v>75</v>
+      </c>
+      <c r="E5" s="13">
         <v>11.0</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="14">
         <v>7.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="7" t="s">
         <v>82</v>
       </c>
+      <c r="B6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="7">
+        <v>75</v>
+      </c>
+      <c r="E6" s="13">
         <v>11.0</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="14">
         <v>7.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="7">
+        <v>75</v>
+      </c>
+      <c r="E7" s="13">
         <v>11.0</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="14">
         <v>7.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="7">
+        <v>75</v>
+      </c>
+      <c r="E8" s="13">
         <v>7.0</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="14">
         <v>8.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="7">
+        <v>89</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="13">
         <v>7.0</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="14">
         <v>8.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="7">
+        <v>88</v>
+      </c>
+      <c r="E10" s="13">
         <v>7.0</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="14">
         <v>8.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="7">
+        <v>88</v>
+      </c>
+      <c r="E11" s="13">
         <v>7.0</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="14">
         <v>8.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="7">
+        <v>88</v>
+      </c>
+      <c r="E12" s="13">
         <v>7.0</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="14">
         <v>8.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="7">
+        <v>88</v>
+      </c>
+      <c r="E13" s="13">
         <v>7.0</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="14">
         <v>8.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="7">
+        <v>88</v>
+      </c>
+      <c r="E14" s="13">
         <v>7.0</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="14">
         <v>8.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="7">
+        <v>88</v>
+      </c>
+      <c r="E15" s="13">
         <v>7.0</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="14">
         <v>8.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="7">
+        <v>103</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="13">
         <v>5.0</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="14">
         <v>9.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="7">
+        <v>102</v>
+      </c>
+      <c r="E17" s="13">
         <v>5.0</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="14">
         <v>9.0</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="7">
+        <v>102</v>
+      </c>
+      <c r="E18" s="13">
         <v>5.0</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="14">
         <v>9.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="7">
+        <v>102</v>
+      </c>
+      <c r="E19" s="13">
         <v>5.0</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="14">
         <v>9.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="7">
+        <v>102</v>
+      </c>
+      <c r="E20" s="13">
         <v>5.0</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="14">
         <v>9.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" s="7">
+        <v>102</v>
+      </c>
+      <c r="E21" s="13">
         <v>5.0</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="14">
         <v>9.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="7">
+        <v>115</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="13">
         <v>3.0</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="14">
         <v>10.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="7">
+        <v>114</v>
+      </c>
+      <c r="E23" s="13">
         <v>3.0</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="14">
         <v>10.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" s="7">
+        <v>114</v>
+      </c>
+      <c r="E24" s="13">
         <v>3.0</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="14">
         <v>10.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="7">
+        <v>114</v>
+      </c>
+      <c r="E25" s="13">
         <v>3.0</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="14">
         <v>10.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E26" s="7">
+        <v>114</v>
+      </c>
+      <c r="E26" s="13">
         <v>3.0</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="14">
         <v>10.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="7">
+        <v>114</v>
+      </c>
+      <c r="E27" s="13">
         <v>3.0</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="14">
         <v>10.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" s="7">
+        <v>126</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="13">
         <v>2.0</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="14">
         <v>11.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" s="7">
+        <v>125</v>
+      </c>
+      <c r="E29" s="13">
         <v>2.0</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="14">
         <v>11.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E30" s="7">
+        <v>125</v>
+      </c>
+      <c r="E30" s="13">
         <v>2.0</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="14">
         <v>11.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E31" s="7">
+        <v>125</v>
+      </c>
+      <c r="E31" s="13">
         <v>2.0</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="14">
         <v>11.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" s="7">
+        <v>125</v>
+      </c>
+      <c r="E32" s="13">
         <v>2.0</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="14">
         <v>11.0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="7">
+        <v>135</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="13">
         <v>1.0</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="14">
         <v>12.0</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E34" s="7">
+        <v>134</v>
+      </c>
+      <c r="E34" s="13">
         <v>1.0</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="14">
         <v>12.0</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E35" s="7">
+        <v>134</v>
+      </c>
+      <c r="E35" s="13">
         <v>1.0</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="14">
         <v>12.0</v>
       </c>
     </row>
@@ -2322,94 +2433,94 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="15" t="s">
         <v>144</v>
       </c>
+      <c r="G1" s="15" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="12">
+      <c r="A2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="18">
         <v>2.7054447E7</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="18">
         <v>1.0</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="13">
+      <c r="D2" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="19">
         <v>55.786</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="19">
         <v>11.468</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="17">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="18">
         <v>2.7054447E7</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="18">
         <v>2.0</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="13">
+      <c r="D3" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="19">
         <v>55.8235758521247</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="19">
         <v>11.4022852800608</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="17">
         <v>36.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="12">
+      <c r="A4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="18">
         <v>2.7054446E7</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="18">
         <v>2.0</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="13">
+      <c r="D4" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="19">
         <v>57.4755132</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="19">
         <v>10.1994273</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="18">
         <v>0.0</v>
       </c>
     </row>
@@ -2447,60 +2558,60 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>70</v>
+      <c r="A1" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="14">
+        <v>159</v>
+      </c>
+      <c r="D2" s="20">
         <v>55.231</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="20">
         <v>10.443</v>
       </c>
       <c r="F2" s="3">
@@ -2510,38 +2621,38 @@
         <v>0.0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I2" s="3">
         <v>60.0</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K2" s="8">
+        <v>161</v>
+      </c>
+      <c r="K2" s="14">
         <v>110.0</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="14">
+        <v>164</v>
+      </c>
+      <c r="D3" s="20">
         <v>55.33131</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="20">
         <v>10.51113</v>
       </c>
       <c r="F3" s="3">
@@ -2551,22 +2662,22 @@
         <v>0.0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I3" s="3">
         <v>90.0</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="K3" s="8">
+        <v>166</v>
+      </c>
+      <c r="K3" s="14">
         <v>100.0</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got Home Kit shirt and shorts fully implemented
</commit_message>
<xml_diff>
--- a/clubs.xlsx
+++ b/clubs.xlsx
@@ -12,13 +12,44 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhyj7qPFZAiGnki/VqkvQL8MtbTyg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7misN4/hp4+ikuUIAH5TOqjdP1E6ug=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="Q1">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAvwfAVtw
+Frederik    (2023-05-02 17:04:20)
+1 to 56</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="N1">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAvwfAVts
+Frederik    (2023-05-02 17:04:09)
+1 to 56</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mh1c/h8BGiEbyBb2GT3odp8SPewBA=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -50,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="191">
   <si>
     <t>Full Name</t>
   </si>
@@ -133,6 +164,12 @@
     <t>Copenhagen, Series 1</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
     <t>Handel Boldklub</t>
   </si>
   <si>
@@ -151,6 +188,12 @@
     <t>932444</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>Club1</t>
   </si>
   <si>
@@ -172,6 +215,12 @@
     <t>Jutland, Series 5</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>Club2</t>
   </si>
   <si>
@@ -184,6 +233,12 @@
     <t>S2A</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>Club3</t>
   </si>
   <si>
@@ -199,6 +254,12 @@
     <t>Zealand, Series 1</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
     <t>Club4</t>
   </si>
   <si>
@@ -208,6 +269,12 @@
     <t>S4</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>Club5</t>
   </si>
   <si>
@@ -217,6 +284,12 @@
     <t>S5</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>Club6</t>
   </si>
   <si>
@@ -226,6 +299,12 @@
     <t>S6</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>Club7</t>
   </si>
   <si>
@@ -235,6 +314,12 @@
     <t>S7</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
     <t>Club8</t>
   </si>
   <si>
@@ -244,6 +329,12 @@
     <t>S8</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>Club9</t>
   </si>
   <si>
@@ -254,6 +345,12 @@
   </si>
   <si>
     <t>Ordrup (Fårevejle)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>Club10</t>
@@ -579,7 +676,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +697,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6D9EEB"/>
+        <bgColor rgb="FF6D9EEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
@@ -608,12 +729,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDEEAF6"/>
         <bgColor rgb="FFDEEAF6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6AA84F"/>
-        <bgColor rgb="FF6AA84F"/>
       </patternFill>
     </fill>
     <fill>
@@ -641,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -660,22 +775,31 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="10" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="11" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -687,19 +811,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1195,114 +1319,126 @@
       <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="4"/>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="8"/>
+      <c r="S2" s="9"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2">
         <v>1912.0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I3" s="3">
         <v>300.0</v>
       </c>
-      <c r="J3" s="6"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="4"/>
       <c r="L3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="8"/>
+      <c r="S3" s="9"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2">
         <v>1875.0</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>37</v>
+      <c r="G4" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I4" s="3">
         <v>2000.0</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" s="8"/>
+      <c r="S4" s="9"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2">
         <v>1838.0</v>
@@ -1311,41 +1447,45 @@
         <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I5" s="3">
         <v>250.0</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="9"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="8"/>
       <c r="L5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="1"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" s="8"/>
+      <c r="S5" s="9"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F6" s="2">
         <v>1801.0</v>
@@ -1354,41 +1494,45 @@
         <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I6" s="3">
         <v>95.0</v>
       </c>
-      <c r="J6" s="6"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="5"/>
       <c r="L6" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="8"/>
+      <c r="S6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2">
         <v>1764.0</v>
@@ -1397,41 +1541,45 @@
         <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I7" s="3">
         <v>90.0</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="8"/>
       <c r="K7" s="5"/>
       <c r="L7" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="O7" s="6"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="6"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="8"/>
+      <c r="S7" s="9"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F8" s="2">
         <v>1727.0</v>
@@ -1440,41 +1588,45 @@
         <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I8" s="3">
         <v>80.0</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="5"/>
       <c r="L8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O8" s="6"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="6"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8" s="8"/>
+      <c r="S8" s="9"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F9" s="2">
         <v>1690.0</v>
@@ -1483,41 +1635,45 @@
         <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I9" s="3">
         <v>78.0</v>
       </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="5"/>
       <c r="L9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="O9" s="6"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="6"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R9" s="8"/>
+      <c r="S9" s="9"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2">
         <v>1653.0</v>
@@ -1526,41 +1682,45 @@
         <v>23</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I10" s="3">
         <v>200.0</v>
       </c>
-      <c r="J10" s="11"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="5"/>
       <c r="L10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="O10" s="6"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="6"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10" s="8"/>
+      <c r="S10" s="9"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2">
         <v>1616.0</v>
@@ -1569,84 +1729,92 @@
         <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I11" s="3">
         <v>120.0</v>
       </c>
-      <c r="J11" s="6"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="5"/>
       <c r="L11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R11" s="8"/>
       <c r="S11" s="9"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F12" s="2">
         <v>1579.0</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>67</v>
+      <c r="G12" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I12" s="3">
         <v>100.0</v>
       </c>
-      <c r="J12" s="11"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="5"/>
       <c r="L12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R12" s="8"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F13" s="2">
         <v>1542.0</v>
@@ -1655,7 +1823,7 @@
         <v>23</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I13" s="3">
         <v>50.0</v>
@@ -1666,22 +1834,27 @@
         <v>25</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="8"/>
       <c r="S13" s="9"/>
     </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1705,62 +1878,62 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>72</v>
+      <c r="C1" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>74</v>
+      <c r="F1" s="15" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="13">
+        <v>98</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="16">
         <v>11.0</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="17">
         <v>7.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>79</v>
+      <c r="A3" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="13">
+        <v>97</v>
+      </c>
+      <c r="E3" s="16">
         <v>11.0</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="17">
         <v>7.0</v>
       </c>
     </row>
@@ -1772,635 +1945,635 @@
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="13">
+        <v>97</v>
+      </c>
+      <c r="E4" s="16">
         <v>11.0</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="17">
         <v>7.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="13">
+        <v>97</v>
+      </c>
+      <c r="E5" s="16">
         <v>11.0</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="17">
         <v>7.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>83</v>
+      <c r="A6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="13">
+        <v>97</v>
+      </c>
+      <c r="E6" s="16">
         <v>11.0</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="17">
         <v>7.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="13">
+        <v>97</v>
+      </c>
+      <c r="E7" s="16">
         <v>11.0</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="17">
         <v>7.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="13">
+        <v>97</v>
+      </c>
+      <c r="E8" s="16">
         <v>7.0</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="17">
         <v>8.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="13">
+        <v>111</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="16">
         <v>7.0</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="17">
         <v>8.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="13">
+        <v>110</v>
+      </c>
+      <c r="E10" s="16">
         <v>7.0</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="17">
         <v>8.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="13">
+        <v>110</v>
+      </c>
+      <c r="E11" s="16">
         <v>7.0</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="17">
         <v>8.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="13">
+        <v>110</v>
+      </c>
+      <c r="E12" s="16">
         <v>7.0</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="17">
         <v>8.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="13">
+        <v>110</v>
+      </c>
+      <c r="E13" s="16">
         <v>7.0</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="17">
         <v>8.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="13">
+        <v>110</v>
+      </c>
+      <c r="E14" s="16">
         <v>7.0</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="17">
         <v>8.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="13">
+        <v>110</v>
+      </c>
+      <c r="E15" s="16">
         <v>7.0</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="17">
         <v>8.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="13">
+        <v>125</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="16">
         <v>5.0</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="17">
         <v>9.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="13">
+        <v>124</v>
+      </c>
+      <c r="E17" s="16">
         <v>5.0</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="17">
         <v>9.0</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="13">
+        <v>124</v>
+      </c>
+      <c r="E18" s="16">
         <v>5.0</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="17">
         <v>9.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="13">
+        <v>124</v>
+      </c>
+      <c r="E19" s="16">
         <v>5.0</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="17">
         <v>9.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="13">
+        <v>124</v>
+      </c>
+      <c r="E20" s="16">
         <v>5.0</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="17">
         <v>9.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="13">
+        <v>124</v>
+      </c>
+      <c r="E21" s="16">
         <v>5.0</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="17">
         <v>9.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="13">
+        <v>137</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="16">
         <v>3.0</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="17">
         <v>10.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="13">
+        <v>136</v>
+      </c>
+      <c r="E23" s="16">
         <v>3.0</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="17">
         <v>10.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E24" s="13">
+        <v>136</v>
+      </c>
+      <c r="E24" s="16">
         <v>3.0</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="17">
         <v>10.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="13">
+        <v>136</v>
+      </c>
+      <c r="E25" s="16">
         <v>3.0</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="17">
         <v>10.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="13">
+        <v>136</v>
+      </c>
+      <c r="E26" s="16">
         <v>3.0</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="17">
         <v>10.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="13">
+        <v>136</v>
+      </c>
+      <c r="E27" s="16">
         <v>3.0</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="17">
         <v>10.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="13">
+        <v>148</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="16">
         <v>2.0</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="17">
         <v>11.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E29" s="13">
+        <v>147</v>
+      </c>
+      <c r="E29" s="16">
         <v>2.0</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="17">
         <v>11.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="13">
+        <v>147</v>
+      </c>
+      <c r="E30" s="16">
         <v>2.0</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="17">
         <v>11.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E31" s="13">
+        <v>147</v>
+      </c>
+      <c r="E31" s="16">
         <v>2.0</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="17">
         <v>11.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" s="13">
+        <v>147</v>
+      </c>
+      <c r="E32" s="16">
         <v>2.0</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="17">
         <v>11.0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="13">
+        <v>157</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="16">
         <v>1.0</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="17">
         <v>12.0</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E34" s="13">
+        <v>156</v>
+      </c>
+      <c r="E34" s="16">
         <v>1.0</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="17">
         <v>12.0</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E35" s="13">
+        <v>156</v>
+      </c>
+      <c r="E35" s="16">
         <v>1.0</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="17">
         <v>12.0</v>
       </c>
     </row>
@@ -2433,94 +2606,94 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>145</v>
+      <c r="A1" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="18">
+      <c r="A2" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="21">
         <v>2.7054447E7</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="21">
         <v>1.0</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="19">
+      <c r="D2" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="22">
         <v>55.786</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="22">
         <v>11.468</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="20">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="18">
+      <c r="A3" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="21">
         <v>2.7054447E7</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="21">
         <v>2.0</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3" s="19">
+      <c r="D3" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="22">
         <v>55.8235758521247</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="22">
         <v>11.4022852800608</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="20">
         <v>36.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="18">
+      <c r="A4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="21">
         <v>2.7054446E7</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="21">
         <v>2.0</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="19">
+      <c r="D4" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="22">
         <v>57.4755132</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="22">
         <v>10.1994273</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="21">
         <v>0.0</v>
       </c>
     </row>
@@ -2558,44 +2731,44 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="12" t="s">
-        <v>71</v>
+      <c r="A1" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2">
@@ -2603,15 +2776,15 @@
         <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" s="20">
+        <v>181</v>
+      </c>
+      <c r="D2" s="23">
         <v>55.231</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="23">
         <v>10.443</v>
       </c>
       <c r="F2" s="3">
@@ -2621,38 +2794,38 @@
         <v>0.0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="I2" s="3">
         <v>60.0</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="14">
+        <v>183</v>
+      </c>
+      <c r="K2" s="17">
         <v>110.0</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D3" s="20">
+        <v>186</v>
+      </c>
+      <c r="D3" s="23">
         <v>55.33131</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="23">
         <v>10.51113</v>
       </c>
       <c r="F3" s="3">
@@ -2662,22 +2835,22 @@
         <v>0.0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="I3" s="3">
         <v>90.0</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="K3" s="14">
+        <v>188</v>
+      </c>
+      <c r="K3" s="17">
         <v>100.0</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fully implemented home kit
</commit_message>
<xml_diff>
--- a/clubs.xlsx
+++ b/clubs.xlsx
@@ -43,7 +43,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mh1c/h8BGiEbyBb2GT3odp8SPewBA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhYHP0cmeroChMtjWPB5FMpnCOkGA=="/>
     </ext>
   </extLst>
 </comments>
@@ -697,8 +697,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
-        <bgColor rgb="FFFF00FF"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -721,12 +721,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDEEAF6"/>
         <bgColor rgb="FFDEEAF6"/>
       </patternFill>
@@ -741,6 +735,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4A86E8"/>
         <bgColor rgb="FF4A86E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -775,7 +775,7 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -799,7 +799,7 @@
     <xf borderId="0" fillId="10" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -817,13 +817,13 @@
     <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1358,7 +1358,7 @@
       <c r="I3" s="3">
         <v>300.0</v>
       </c>
-      <c r="J3" s="11"/>
+      <c r="J3" s="6"/>
       <c r="K3" s="4"/>
       <c r="L3" s="1" t="s">
         <v>26</v>
@@ -1369,8 +1369,8 @@
       <c r="N3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="5"/>
       <c r="Q3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="F4" s="2">
         <v>1875.0</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1406,7 +1406,7 @@
         <v>2000.0</v>
       </c>
       <c r="J4" s="8"/>
-      <c r="K4" s="13"/>
+      <c r="K4" s="12"/>
       <c r="L4" s="1" t="s">
         <v>43</v>
       </c>
@@ -1416,8 +1416,8 @@
       <c r="N4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="7"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="12"/>
       <c r="Q4" s="1" t="s">
         <v>45</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="I5" s="3">
         <v>250.0</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="J5" s="13"/>
       <c r="K5" s="8"/>
       <c r="L5" s="1" t="s">
         <v>25</v>
@@ -1463,8 +1463,8 @@
       <c r="N5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="I6" s="3">
         <v>95.0</v>
       </c>
-      <c r="J6" s="11"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="5"/>
       <c r="L6" s="1" t="s">
         <v>56</v>
@@ -1510,7 +1510,7 @@
       <c r="N6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="6"/>
+      <c r="O6" s="5"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="1" t="s">
         <v>58</v>
@@ -1558,7 +1558,7 @@
         <v>62</v>
       </c>
       <c r="O7" s="6"/>
-      <c r="P7" s="7"/>
+      <c r="P7" s="5"/>
       <c r="Q7" s="1" t="s">
         <v>63</v>
       </c>
@@ -1593,7 +1593,7 @@
       <c r="I8" s="3">
         <v>80.0</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="5"/>
       <c r="L8" s="1" t="s">
         <v>25</v>
@@ -1604,8 +1604,8 @@
       <c r="N8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="7"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="6"/>
       <c r="Q8" s="1" t="s">
         <v>68</v>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="I9" s="3">
         <v>78.0</v>
       </c>
-      <c r="J9" s="11"/>
+      <c r="J9" s="6"/>
       <c r="K9" s="5"/>
       <c r="L9" s="1" t="s">
         <v>34</v>
@@ -1652,7 +1652,7 @@
         <v>72</v>
       </c>
       <c r="O9" s="6"/>
-      <c r="P9" s="7"/>
+      <c r="P9" s="14"/>
       <c r="Q9" s="1" t="s">
         <v>73</v>
       </c>
@@ -1687,7 +1687,7 @@
       <c r="I10" s="3">
         <v>200.0</v>
       </c>
-      <c r="J10" s="14"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="5"/>
       <c r="L10" s="1" t="s">
         <v>25</v>
@@ -1698,7 +1698,7 @@
       <c r="N10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="6"/>
+      <c r="O10" s="14"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="1" t="s">
         <v>78</v>
@@ -1734,7 +1734,7 @@
       <c r="I11" s="3">
         <v>120.0</v>
       </c>
-      <c r="J11" s="11"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="5"/>
       <c r="L11" s="1" t="s">
         <v>26</v>
@@ -1745,7 +1745,7 @@
       <c r="N11" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O11" s="6"/>
+      <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="1" t="s">
         <v>83</v>
@@ -1772,7 +1772,7 @@
       <c r="F12" s="2">
         <v>1579.0</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>87</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1781,7 +1781,7 @@
       <c r="I12" s="3">
         <v>100.0</v>
       </c>
-      <c r="J12" s="14"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="5"/>
       <c r="L12" s="1" t="s">
         <v>25</v>
@@ -1792,8 +1792,8 @@
       <c r="N12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="7"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
       <c r="Q12" s="1" t="s">
         <v>89</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>28</v>
       </c>
       <c r="O13" s="6"/>
-      <c r="P13" s="7"/>
+      <c r="P13" s="6"/>
       <c r="Q13" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Fully implemented away kits
</commit_message>
<xml_diff>
--- a/clubs.xlsx
+++ b/clubs.xlsx
@@ -676,7 +676,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -715,12 +715,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDEEAF6"/>
         <bgColor rgb="FFDEEAF6"/>
       </patternFill>
@@ -745,6 +739,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE69138"/>
+        <bgColor rgb="FFE69138"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
       </patternFill>
@@ -756,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -784,11 +790,11 @@
     <xf borderId="0" fillId="6" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -796,10 +802,13 @@
     <xf borderId="0" fillId="9" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -811,19 +820,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1328,16 +1337,16 @@
         <v>28</v>
       </c>
       <c r="R2" s="8"/>
-      <c r="S2" s="9"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1374,8 +1383,8 @@
       <c r="Q3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="9"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -1396,7 +1405,7 @@
       <c r="F4" s="2">
         <v>1875.0</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1406,7 +1415,7 @@
         <v>2000.0</v>
       </c>
       <c r="J4" s="8"/>
-      <c r="K4" s="12"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="1" t="s">
         <v>43</v>
       </c>
@@ -1417,12 +1426,12 @@
         <v>44</v>
       </c>
       <c r="O4" s="8"/>
-      <c r="P4" s="12"/>
+      <c r="P4" s="11"/>
       <c r="Q4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="9"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="6"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -1452,7 +1461,7 @@
       <c r="I5" s="3">
         <v>250.0</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="8"/>
       <c r="L5" s="1" t="s">
         <v>25</v>
@@ -1463,13 +1472,13 @@
       <c r="N5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="13"/>
+      <c r="O5" s="12"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R5" s="8"/>
-      <c r="S5" s="9"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -1516,7 +1525,7 @@
         <v>58</v>
       </c>
       <c r="R6" s="8"/>
-      <c r="S6" s="9"/>
+      <c r="S6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
@@ -1562,8 +1571,8 @@
       <c r="Q7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R7" s="8"/>
-      <c r="S7" s="9"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
@@ -1593,7 +1602,7 @@
       <c r="I8" s="3">
         <v>80.0</v>
       </c>
-      <c r="J8" s="13"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="5"/>
       <c r="L8" s="1" t="s">
         <v>25</v>
@@ -1604,13 +1613,13 @@
       <c r="N8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O8" s="14"/>
+      <c r="O8" s="13"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R8" s="8"/>
-      <c r="S8" s="9"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="13"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -1652,12 +1661,12 @@
         <v>72</v>
       </c>
       <c r="O9" s="6"/>
-      <c r="P9" s="14"/>
+      <c r="P9" s="13"/>
       <c r="Q9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R9" s="8"/>
-      <c r="S9" s="9"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -1687,7 +1696,7 @@
       <c r="I10" s="3">
         <v>200.0</v>
       </c>
-      <c r="J10" s="13"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="5"/>
       <c r="L10" s="1" t="s">
         <v>25</v>
@@ -1698,13 +1707,13 @@
       <c r="N10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="14"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R10" s="8"/>
-      <c r="S10" s="9"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -1750,8 +1759,8 @@
       <c r="Q11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="R11" s="8"/>
-      <c r="S11" s="9"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="11"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
@@ -1772,7 +1781,7 @@
       <c r="F12" s="2">
         <v>1579.0</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>87</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1781,7 +1790,7 @@
       <c r="I12" s="3">
         <v>100.0</v>
       </c>
-      <c r="J12" s="13"/>
+      <c r="J12" s="12"/>
       <c r="K12" s="5"/>
       <c r="L12" s="1" t="s">
         <v>25</v>
@@ -1797,8 +1806,8 @@
       <c r="Q12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="R12" s="8"/>
-      <c r="S12" s="9"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="14"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
@@ -1844,8 +1853,8 @@
       <c r="Q13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R13" s="8"/>
-      <c r="S13" s="9"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="15"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -1878,22 +1887,22 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>94</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1907,33 +1916,33 @@
       <c r="C2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="17">
         <v>11.0</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="18">
         <v>7.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="17">
         <v>11.0</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="18">
         <v>7.0</v>
       </c>
     </row>
@@ -1950,10 +1959,10 @@
       <c r="D4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="17">
         <v>11.0</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="18">
         <v>7.0</v>
       </c>
     </row>
@@ -1970,30 +1979,30 @@
       <c r="D5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="17">
         <v>11.0</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="18">
         <v>7.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="17">
         <v>11.0</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="18">
         <v>7.0</v>
       </c>
     </row>
@@ -2010,10 +2019,10 @@
       <c r="D7" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="17">
         <v>11.0</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="18">
         <v>7.0</v>
       </c>
     </row>
@@ -2030,10 +2039,10 @@
       <c r="D8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="17">
         <v>7.0</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="18">
         <v>8.0</v>
       </c>
     </row>
@@ -2047,13 +2056,13 @@
       <c r="C9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="17">
         <v>7.0</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="18">
         <v>8.0</v>
       </c>
     </row>
@@ -2070,10 +2079,10 @@
       <c r="D10" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="17">
         <v>7.0</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="18">
         <v>8.0</v>
       </c>
     </row>
@@ -2090,10 +2099,10 @@
       <c r="D11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="17">
         <v>7.0</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="18">
         <v>8.0</v>
       </c>
     </row>
@@ -2110,10 +2119,10 @@
       <c r="D12" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="17">
         <v>7.0</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="18">
         <v>8.0</v>
       </c>
     </row>
@@ -2130,10 +2139,10 @@
       <c r="D13" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="17">
         <v>7.0</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="18">
         <v>8.0</v>
       </c>
     </row>
@@ -2150,10 +2159,10 @@
       <c r="D14" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="17">
         <v>7.0</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="18">
         <v>8.0</v>
       </c>
     </row>
@@ -2170,10 +2179,10 @@
       <c r="D15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="17">
         <v>7.0</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="18">
         <v>8.0</v>
       </c>
     </row>
@@ -2187,13 +2196,13 @@
       <c r="C16" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="17">
         <v>5.0</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="18">
         <v>9.0</v>
       </c>
     </row>
@@ -2210,10 +2219,10 @@
       <c r="D17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="17">
         <v>5.0</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="18">
         <v>9.0</v>
       </c>
     </row>
@@ -2230,10 +2239,10 @@
       <c r="D18" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="17">
         <v>5.0</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="18">
         <v>9.0</v>
       </c>
     </row>
@@ -2250,10 +2259,10 @@
       <c r="D19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="17">
         <v>5.0</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="18">
         <v>9.0</v>
       </c>
     </row>
@@ -2270,10 +2279,10 @@
       <c r="D20" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="17">
         <v>5.0</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="18">
         <v>9.0</v>
       </c>
     </row>
@@ -2290,10 +2299,10 @@
       <c r="D21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="17">
         <v>5.0</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="18">
         <v>9.0</v>
       </c>
     </row>
@@ -2307,13 +2316,13 @@
       <c r="C22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="17">
         <v>3.0</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="18">
         <v>10.0</v>
       </c>
     </row>
@@ -2330,10 +2339,10 @@
       <c r="D23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="17">
         <v>3.0</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="18">
         <v>10.0</v>
       </c>
     </row>
@@ -2350,10 +2359,10 @@
       <c r="D24" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="17">
         <v>3.0</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="18">
         <v>10.0</v>
       </c>
     </row>
@@ -2370,10 +2379,10 @@
       <c r="D25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="17">
         <v>3.0</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="18">
         <v>10.0</v>
       </c>
     </row>
@@ -2390,10 +2399,10 @@
       <c r="D26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="17">
         <v>3.0</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="18">
         <v>10.0</v>
       </c>
     </row>
@@ -2410,10 +2419,10 @@
       <c r="D27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="17">
         <v>3.0</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="18">
         <v>10.0</v>
       </c>
     </row>
@@ -2427,13 +2436,13 @@
       <c r="C28" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="17">
         <v>2.0</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="18">
         <v>11.0</v>
       </c>
     </row>
@@ -2450,10 +2459,10 @@
       <c r="D29" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="17">
         <v>2.0</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F29" s="18">
         <v>11.0</v>
       </c>
     </row>
@@ -2470,10 +2479,10 @@
       <c r="D30" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="17">
         <v>2.0</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="18">
         <v>11.0</v>
       </c>
     </row>
@@ -2490,10 +2499,10 @@
       <c r="D31" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="17">
         <v>2.0</v>
       </c>
-      <c r="F31" s="17">
+      <c r="F31" s="18">
         <v>11.0</v>
       </c>
     </row>
@@ -2510,10 +2519,10 @@
       <c r="D32" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="17">
         <v>2.0</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="18">
         <v>11.0</v>
       </c>
     </row>
@@ -2527,13 +2536,13 @@
       <c r="C33" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="17">
         <v>1.0</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F33" s="18">
         <v>12.0</v>
       </c>
     </row>
@@ -2550,10 +2559,10 @@
       <c r="D34" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="17">
         <v>1.0</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="18">
         <v>12.0</v>
       </c>
     </row>
@@ -2570,10 +2579,10 @@
       <c r="D35" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="17">
         <v>1.0</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F35" s="18">
         <v>12.0</v>
       </c>
     </row>
@@ -2606,94 +2615,94 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="22">
         <v>2.7054447E7</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="22">
         <v>1.0</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="23">
         <v>55.786</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="23">
         <v>11.468</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="21">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="22">
         <v>2.7054447E7</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="22">
         <v>2.0</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="23">
         <v>55.8235758521247</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="23">
         <v>11.4022852800608</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="21">
         <v>36.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="22">
         <v>2.7054446E7</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="22">
         <v>2.0</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="23">
         <v>57.4755132</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="23">
         <v>10.1994273</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="22">
         <v>0.0</v>
       </c>
     </row>
@@ -2731,7 +2740,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -2781,10 +2790,10 @@
       <c r="C2" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="24">
         <v>55.231</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="24">
         <v>10.443</v>
       </c>
       <c r="F2" s="3">
@@ -2802,7 +2811,7 @@
       <c r="J2" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="17">
+      <c r="K2" s="18">
         <v>110.0</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -2822,10 +2831,10 @@
       <c r="C3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>55.33131</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>10.51113</v>
       </c>
       <c r="F3" s="3">
@@ -2843,7 +2852,7 @@
       <c r="J3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="18">
         <v>100.0</v>
       </c>
       <c r="L3" s="3" t="s">

</xml_diff>